<commit_message>
modified:   ../../../../bank/pout-2022-09-30.xlsx yt_new file:   yt_Preach.js yt_modified:   yt_data.js
</commit_message>
<xml_diff>
--- a/bank/pout-2022-09-30.xlsx
+++ b/bank/pout-2022-09-30.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weiding/Sites/weidroot/weidroot_2017-01-06/app/github/wdingsoft/whingd/bank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8B69BA-E35A-2E44-9146-92B9671CA292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEB3B68-7D8B-5F4E-A54A-6050A718CFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="12880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="5560" windowWidth="25600" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expense-Log" sheetId="6" r:id="rId1"/>
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="145">
   <si>
     <t>22-06-26</t>
   </si>
@@ -660,6 +660,12 @@
   </si>
   <si>
     <t>Income(Y)</t>
+  </si>
+  <si>
+    <t>22-10-11</t>
+  </si>
+  <si>
+    <t>Identical Ideneity In Passport (Emily)</t>
   </si>
 </sst>
 </file>
@@ -811,7 +817,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1004,13 +1010,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1161,6 +1178,7 @@
     <xf numFmtId="43" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1380,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED1393D-93E0-6547-BE37-37C21B49335F}">
   <dimension ref="A1:N164"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="E123" sqref="E123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2804,16 +2822,23 @@
       <c r="F121" s="35"/>
     </row>
     <row r="122" spans="2:9" s="81" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B122" s="35"/>
+      <c r="B122" s="21"/>
       <c r="C122" s="35"/>
       <c r="D122" s="45"/>
       <c r="E122" s="35"/>
       <c r="F122" s="35"/>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B123" s="21"/>
-      <c r="C123" s="34"/>
-      <c r="E123" s="21"/>
+      <c r="B123" s="83" t="s">
+        <v>143</v>
+      </c>
+      <c r="C123" s="23"/>
+      <c r="D123" s="4">
+        <v>-260</v>
+      </c>
+      <c r="E123" s="21" t="s">
+        <v>144</v>
+      </c>
       <c r="F123" s="21"/>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.15">
@@ -3072,7 +3097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EBE6AC8-509B-A643-BB19-E41D6E7661ED}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>